<commit_message>
added mount for blade :weary:
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ZEDD-VALORANT-SWORD-thingy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F905FB-14E8-4BB0-BFD1-AA1BE386227A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A7C2CD-75BE-4247-8B7D-9A96367587BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2CDE34C8-BA9E-46B6-BD57-4968B0C3BB9C}</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{2CDE34C8-BA9E-46B6-BD57-4968B0C3BB9C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    could even use a dollarama power bank</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
@@ -73,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +121,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,6 +173,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jahangir Abdullayev" id="{FB0ED26D-D91C-4ABD-86A9-2D945EA8C290}" userId="2627344c419a245c" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,12 +442,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B5" dT="2021-11-10T02:23:04.90" personId="{FB0ED26D-D91C-4ABD-86A9-2D945EA8C290}" id="{2CDE34C8-BA9E-46B6-BD57-4968B0C3BB9C}">
+    <text>could even use a dollarama power bank</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,5 +578,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>